<commit_message>
Gameplay Completed (Missing Shield)
</commit_message>
<xml_diff>
--- a/ReportsAndOthers/Reports/Detail_Planner.xlsx
+++ b/ReportsAndOthers/Reports/Detail_Planner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LEIM\Unity\UnityMobileGame\ReportsAndOthers\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E0D2FE-F82A-4DC1-98BD-4D68CDBB248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CB8CA-5226-492E-91A9-551B9723B1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A08252EC-0269-49E2-A171-BD9FBC0249CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Deploy</t>
+  </si>
+  <si>
+    <t>Status Effect Mechanic</t>
   </si>
 </sst>
 </file>
@@ -182,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -331,13 +340,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -374,9 +384,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,8 +393,19 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="20% - Cor4" xfId="4" builtinId="42"/>
     <cellStyle name="40% - Cor1" xfId="2" builtinId="31"/>
     <cellStyle name="Correto" xfId="1" builtinId="26"/>
     <cellStyle name="Neutro" xfId="3" builtinId="28"/>
@@ -703,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58694E3-0194-4E98-8BC1-9E7249C074C6}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,29 +734,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -789,7 +807,7 @@
       <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -813,7 +831,9 @@
       <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -853,7 +873,7 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2"/>
@@ -876,7 +896,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2"/>
@@ -923,7 +943,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="2"/>
@@ -947,7 +967,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="2"/>
@@ -971,7 +991,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="2"/>
@@ -994,7 +1014,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="2"/>
@@ -1010,54 +1030,44 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="G12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="G13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1066,7 +1076,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
@@ -1074,13 +1084,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="H14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1091,7 +1099,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="2"/>
@@ -1100,14 +1108,14 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1116,7 +1124,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
@@ -1127,25 +1135,21 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="K16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="2"/>
@@ -1157,18 +1161,24 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="L17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="2"/>
@@ -1191,7 +1201,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -1203,10 +1213,10 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="L19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -1214,7 +1224,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
@@ -1227,17 +1237,17 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="M20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="2"/>
@@ -1251,88 +1261,78 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="N21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q22" s="14" t="s">
-        <v>11</v>
-      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q23" s="10"/>
+      <c r="H23" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="2"/>
@@ -1346,7 +1346,9 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="O24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1357,7 +1359,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
@@ -1372,13 +1374,18 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="O25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1394,7 +1401,9 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="10"/>
+      <c r="Q26" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
@@ -1469,22 +1478,40 @@
       <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="12"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Gameplay and Small World Generation  (#2)
* Enemy generated dynamically

* Mana

* Fixed Collider hitboxes

* Update SampleScene.unity

* GenerateAttacksFromJSON

* EnemyAI - Implemented not polished

* interface and qoe enemies changes

* Fixed attacks bugs and Added HealthBar UI

* Gameplay Completed (Missing Shield)

* Shield Gameplay
</commit_message>
<xml_diff>
--- a/ReportsAndOthers/Reports/Detail_Planner.xlsx
+++ b/ReportsAndOthers/Reports/Detail_Planner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LEIM\Unity\UnityMobileGame\ReportsAndOthers\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77464E93-0BE2-4585-97F9-2B7C07C7CE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8CB8CA-5226-492E-91A9-551B9723B1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A08252EC-0269-49E2-A171-BD9FBC0249CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Deploy</t>
+  </si>
+  <si>
+    <t>Status Effect Mechanic</t>
   </si>
 </sst>
 </file>
@@ -176,13 +179,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,17 +205,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -315,14 +324,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -350,26 +375,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="40% - Cor1" xfId="3" builtinId="31"/>
+  <cellStyles count="5">
+    <cellStyle name="20% - Cor4" xfId="4" builtinId="42"/>
+    <cellStyle name="40% - Cor1" xfId="2" builtinId="31"/>
     <cellStyle name="Correto" xfId="1" builtinId="26"/>
-    <cellStyle name="Entrada" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58694E3-0194-4E98-8BC1-9E7249C074C6}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10:U11"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,29 +734,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -768,7 +807,7 @@
       <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -777,22 +816,24 @@
         <v>20</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="5"/>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -808,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2"/>
@@ -832,7 +873,7 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2"/>
@@ -879,7 +920,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2"/>
@@ -902,7 +943,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="2"/>
@@ -926,7 +967,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="2"/>
@@ -950,7 +991,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="2"/>
@@ -973,7 +1014,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="2"/>
@@ -989,54 +1030,44 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="G12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="G13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1045,7 +1076,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
@@ -1053,13 +1084,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="H14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -1070,7 +1099,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="2"/>
@@ -1079,14 +1108,14 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1095,7 +1124,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
@@ -1106,25 +1135,21 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="K16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="2"/>
@@ -1136,18 +1161,24 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="L17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="2"/>
@@ -1170,7 +1201,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -1182,10 +1213,10 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="L19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -1193,7 +1224,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
@@ -1206,17 +1237,17 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="M20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="2"/>
@@ -1230,88 +1261,78 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="N21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="N22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q22" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q23" s="10"/>
+      <c r="H23" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="2"/>
@@ -1325,7 +1346,9 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="O24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1336,7 +1359,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
@@ -1351,13 +1374,18 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="O25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1373,7 +1401,9 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="10"/>
+      <c r="Q26" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
@@ -1448,22 +1478,40 @@
       <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="12"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="10"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>